<commit_message>
feat: first stable version with UI fixes
</commit_message>
<xml_diff>
--- a/assets/medpredict_template.xlsx
+++ b/assets/medpredict_template.xlsx
@@ -1,124 +1,142 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4a649c208c0aef3/Biomed/PFE/Microscope PROVIDO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28C10CE-C95D-482E-82DF-9F2DE6FC7130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7283478-5858-4DB1-812B-47C7A6F80888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="logs" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+  <si>
+    <t>ID_événement</t>
+  </si>
+  <si>
+    <t>Module_ID</t>
+  </si>
+  <si>
+    <t>Durée(h)</t>
+  </si>
+  <si>
+    <t>C (Criticité)</t>
+  </si>
+  <si>
+    <t>G (Gravité)</t>
+  </si>
+  <si>
+    <t>O (Occurrence)</t>
+  </si>
+  <si>
+    <t>D (Détectabilité)</t>
+  </si>
+  <si>
+    <t>MTBF (h)</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Module_concerné</t>
+  </si>
   <si>
     <t>timestamp</t>
   </si>
   <si>
-    <t>equipment_name</t>
-  </si>
-  <si>
-    <t>module</t>
-  </si>
-  <si>
-    <t>Module_ID</t>
-  </si>
-  <si>
-    <t>ID_événement</t>
-  </si>
-  <si>
-    <t>Durée(h)</t>
-  </si>
-  <si>
-    <t>C (Criticité)</t>
-  </si>
-  <si>
-    <t>G (Gravité)</t>
-  </si>
-  <si>
-    <t>O (Occurrence)</t>
-  </si>
-  <si>
-    <t>D (Détectabilité)</t>
-  </si>
-  <si>
-    <t>MTBF (h)</t>
-  </si>
-  <si>
-    <t>Label Feature</t>
-  </si>
-  <si>
-    <t>severity</t>
-  </si>
-  <si>
-    <t>anomaly_score</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>2025-08-21 09:41:02</t>
-  </si>
-  <si>
-    <t>Microscope chirurgical ORL</t>
-  </si>
-  <si>
-    <t>Laser module</t>
-  </si>
-  <si>
-    <t>E00001</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Periodic calibration complete</t>
-  </si>
-  <si>
-    <t>2025-08-21 10:12:45</t>
-  </si>
-  <si>
-    <t>Cartes EEPROM</t>
-  </si>
-  <si>
-    <t>E00024</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Overheating sensor triggered near power supply</t>
-  </si>
-  <si>
-    <t>2025-08-21 11:03:09</t>
-  </si>
-  <si>
-    <t>Alimentation</t>
-  </si>
-  <si>
-    <t>E00003</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Voltage ripple within tolerance</t>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>binary_label</t>
+  </si>
+  <si>
+    <t>window_index</t>
+  </si>
+  <si>
+    <t>window_start</t>
+  </si>
+  <si>
+    <t>window_end</t>
+  </si>
+  <si>
+    <t>window_label</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>E28065</t>
+  </si>
+  <si>
+    <t>E42316</t>
+  </si>
+  <si>
+    <t>E73181</t>
+  </si>
+  <si>
+    <t>E76478</t>
+  </si>
+  <si>
+    <t>XY Control</t>
+  </si>
+  <si>
+    <t>Diagnostic carte / EEPROM</t>
+  </si>
+  <si>
+    <t>Light System</t>
+  </si>
+  <si>
+    <t>2025-07-22 03:01:40</t>
+  </si>
+  <si>
+    <t>2025-06-30 16:54:21</t>
+  </si>
+  <si>
+    <t>2025-07-22 04:07:40</t>
+  </si>
+  <si>
+    <t>2025-06-30 18:13:21</t>
+  </si>
+  <si>
+    <t>2025-07-22 02:11:05</t>
+  </si>
+  <si>
+    <t>2025-06-30 15:17:56</t>
+  </si>
+  <si>
+    <t>2025-07-22 07:12:46</t>
+  </si>
+  <si>
+    <t>2025-06-30 20:19:47</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,7 +148,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,11 +189,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,9 +213,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -231,7 +253,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -265,6 +287,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -299,9 +322,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,32 +499,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="48.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,149 +569,256 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>916.17456949740404</v>
       </c>
       <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>4913.26</v>
+        <v>2</v>
       </c>
       <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3795.7107700000001</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2">
+        <v>45599.945902777778</v>
+      </c>
+      <c r="L2" s="2">
+        <v>45599.945902777778</v>
+      </c>
+      <c r="M2" s="2">
+        <v>45600.582135115743</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>6131</v>
+      </c>
+      <c r="P2" s="2">
+        <v>45599.938171296293</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>45599.979837962957</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>81</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>2644.5321800000002</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="2">
+        <v>45707.179062499999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>45707.179062499999</v>
+      </c>
+      <c r="M3" s="2">
+        <v>45707.179409722223</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>16426</v>
+      </c>
+      <c r="P3" s="2">
+        <v>45707.177754629629</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>45707.219421296293</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>274.06018</v>
+      </c>
+      <c r="D4">
+        <v>96</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>1587.9577999999999</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
         <v>26</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>2116.64</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2">
-        <v>0.12</v>
-      </c>
-      <c r="O2" t="s">
-        <v>20</v>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>294</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="D3">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>699.58557299999995</v>
+      </c>
+      <c r="D5">
+        <v>120</v>
+      </c>
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3">
-        <v>2581.29</v>
-      </c>
-      <c r="G3">
-        <v>129</v>
-      </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-      <c r="I3">
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>1308.4000000000001</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3">
-        <v>0.87</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="H5">
+        <v>1234.10186</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="K5" t="s">
         <v>27</v>
       </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4">
-        <v>808.27</v>
-      </c>
-      <c r="G4">
-        <v>16</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>4767.7700000000004</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
         <v>29</v>
       </c>
-      <c r="N4">
-        <v>0.35</v>
-      </c>
-      <c r="O4" t="s">
-        <v>30</v>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>255</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>